<commit_message>
Code refactoring and repackaging
</commit_message>
<xml_diff>
--- a/examples/Australia OGD/go_card_retailers/counters_summary.xlsx
+++ b/examples/Australia OGD/go_card_retailers/counters_summary.xlsx
@@ -466,10 +466,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -490,16 +490,16 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.001122</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -533,10 +533,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -557,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001122</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -667,10 +667,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -734,10 +734,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -788,10 +788,10 @@
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -801,10 +801,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -855,10 +855,10 @@
         <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -892,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -935,10 +935,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -959,10 +959,10 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
@@ -1002,10 +1002,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.003367</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -1163,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>0.001122</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
@@ -1230,7 +1230,7 @@
         <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>0.001122</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>0.001122</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
         <v>0</v>
@@ -1364,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>0.001122</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>0.001122</v>
+        <v>0</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
@@ -1498,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>0.001122</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
@@ -1562,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
@@ -1696,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>

</xml_diff>